<commit_message>
1st version of Bayesian learning finished
</commit_message>
<xml_diff>
--- a/data/wateredges.xlsx
+++ b/data/wateredges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/yu_wang_1_vanderbilt_edu/Documents/code/Infrastructure-network-simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/yu_wang_1_vanderbilt_edu/Documents/code/Bayesian_Inference/Bayesian_Graph_Learning_2.0/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{412F8916-D870-449F-BCD5-A55BA05123E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AF9F2FA-31A9-4DBD-9818-7EE7FA4AF3DD}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{412F8916-D870-449F-BCD5-A55BA05123E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{839FED35-CA72-4D3E-85FD-C43BC60A1437}"/>
   <bookViews>
-    <workbookView xWindow="-4237" yWindow="1028" windowWidth="9045" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,19 +354,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.265625" customWidth="1"/>
-    <col min="3" max="3" width="35.3984375" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -378,7 +378,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -390,7 +390,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -402,7 +402,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -414,7 +414,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -426,7 +426,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -438,7 +438,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -450,7 +450,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -462,7 +462,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -474,7 +474,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -486,7 +486,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -498,7 +498,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -510,7 +510,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -522,7 +522,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -534,7 +534,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -546,7 +546,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -558,7 +558,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -570,7 +570,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -582,7 +582,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -594,7 +594,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -606,7 +606,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -618,7 +618,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -630,7 +630,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -642,7 +642,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -654,7 +654,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -666,7 +666,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -678,7 +678,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -690,7 +690,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -702,7 +702,7 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -714,7 +714,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -726,7 +726,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -738,7 +738,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -750,7 +750,7 @@
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -762,7 +762,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -774,7 +774,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -786,7 +786,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -798,7 +798,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -810,7 +810,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -822,7 +822,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -834,7 +834,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -846,7 +846,7 @@
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -858,7 +858,7 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -882,7 +882,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -894,7 +894,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -906,7 +906,7 @@
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -918,7 +918,7 @@
       </c>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -930,7 +930,7 @@
       </c>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -942,7 +942,7 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -954,7 +954,7 @@
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -966,7 +966,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -978,7 +978,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -990,7 +990,7 @@
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -1218,8 +1218,50 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
+        <v>3</v>
+      </c>
+      <c r="C72" s="1">
+        <v>11</v>
+      </c>
       <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
+        <v>11</v>
+      </c>
+      <c r="C73" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
+        <v>9</v>
+      </c>
+      <c r="C74" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1">
+        <v>13</v>
+      </c>
+      <c r="C75" s="1">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>